<commit_message>
Valor total CLP impreso en Consola Version Run en Edge
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,12 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Prop Destacada 0,95 UF</t>
   </si>
   <si>
     <t>$ 27.323 CLP 17-10-20</t>
+  </si>
+  <si>
+    <t>$ 27.333 CLP 19-10-20</t>
   </si>
 </sst>
 </file>
@@ -392,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -423,6 +426,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Version Run en FIREFOX
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="6">
   <si>
     <t>Prop Destacada 0,95 UF</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>$ 27.333 CLP 19-10-20</t>
+  </si>
+  <si>
+    <t>$ 27.339 CLP 20-10-20</t>
+  </si>
+  <si>
+    <t>$ 27.344 CLP 21-10-20</t>
+  </si>
+  <si>
+    <t>$ 27.354 CLP 23-10-20</t>
   </si>
 </sst>
 </file>
@@ -395,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -436,6 +445,71 @@
         <v>2</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modificación de escenario e incorporación de config.properties
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="8">
   <si>
     <t>Prop Destacada 0,95 UF</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>$ 27.354 CLP 23-10-20</t>
+  </si>
+  <si>
+    <t>$ 27.381 CLP 28-10-20</t>
+  </si>
+  <si>
+    <t>$ 27.386 CLP 29-10-20</t>
   </si>
 </sst>
 </file>
@@ -404,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -510,6 +516,131 @@
         <v>5</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modificación de escenario e incorporación de config.properties Flujo Producto
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="8">
   <si>
     <t>Prop Destacada 0,95 UF</t>
   </si>
@@ -410,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A44"/>
+  <dimension ref="A1:A46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -641,6 +641,16 @@
         <v>7</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambio en la Class login
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="11">
   <si>
     <t>Prop Destacada 0,95 UF</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>$ 27.391 CLP 30-10-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 03-11-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 06-11-20</t>
   </si>
 </sst>
 </file>
@@ -413,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A52"/>
+  <dimension ref="A1:A54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -684,6 +690,16 @@
         <v>8</v>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambion en la clase login
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="11">
   <si>
     <t>Prop Destacada 0,95 UF</t>
   </si>
@@ -419,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A54"/>
+  <dimension ref="A1:A55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -700,6 +700,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización de archivo Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="12">
   <si>
     <t>Prop Destacada 0,95 UF</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 06-11-20</t>
+  </si>
+  <si>
+    <t>$ 17.323 CLP 06-11-20</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A55"/>
+  <dimension ref="A1:A57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -705,6 +708,16 @@
         <v>10</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Flujo de datos de Planes y Productos (Intellij Idea)
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhurtado\Documents\QA Gestion Corredor\Toctoc_QA_Gestion_Corredor\src\test\resources\filepath\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F23D2A5-3D53-431A-9AFB-0B83EE371C1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2531B6-6D7C-4BC9-A272-BCBC4859DBA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1A15881D-BF6E-4E61-BDC0-2AE68B47EA9A}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="12">
-  <si>
-    <t>Prop Destacada 0,95 UF</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="16">
   <si>
     <t>$ 27.323 CLP 17-10-20</t>
   </si>
@@ -70,13 +67,27 @@
   </si>
   <si>
     <t>$ 17.323 CLP 06-11-20</t>
+  </si>
+  <si>
+    <t>TOTAL: 09-11-20</t>
+  </si>
+  <si>
+    <t>$ 27.444 CLP 09-11-20</t>
+  </si>
+  <si>
+    <t>$ 34.386 CLP 10-11-20</t>
+  </si>
+  <si>
+    <t>$ 27.451 CLP 10-11-20</t>
+  </si>
+  <si>
+    <t>Prop Destacada 0,95 UF / Plan Inicia 1,19 UF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -422,300 +433,340 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A57"/>
+  <dimension ref="A1:A65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="1" max="1" width="38.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Flujo de datos de Productos (Intellij Idea)
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhurtado\Documents\QA Gestion Corredor\Toctoc_QA_Gestion_Corredor\src\test\resources\filepath\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="17">
   <si>
     <t>$ 27.323 CLP 17-10-20</t>
   </si>
@@ -82,12 +82,16 @@
   </si>
   <si>
     <t>Prop Destacada 0,95 UF / Plan Inicia 1,19 UF</t>
+  </si>
+  <si>
+    <t>$ 27.457 CLP 11-11-20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -433,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A65"/>
+  <dimension ref="A1:A67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -441,7 +445,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="38.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -769,6 +773,16 @@
         <v>14</v>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Flujo de datos de Productos (Jenkins)
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="24">
   <si>
     <t>$ 27.323 CLP 17-10-20</t>
   </si>
@@ -85,6 +85,27 @@
   </si>
   <si>
     <t>$ 27.457 CLP 11-11-20</t>
+  </si>
+  <si>
+    <t>$ 27.489 CLP 16-11-20</t>
+  </si>
+  <si>
+    <t>$ 34.434 CLP 16-11-20</t>
+  </si>
+  <si>
+    <t>$ 27.495 CLP 17-11-20</t>
+  </si>
+  <si>
+    <t>$ 34.442 CLP 17-11-20</t>
+  </si>
+  <si>
+    <t>$ 34.458 CLP 19-11-20</t>
+  </si>
+  <si>
+    <t>$ 27.508 CLP 19-11-20</t>
+  </si>
+  <si>
+    <t>$ 27.515 CLP 20-11-20</t>
   </si>
 </sst>
 </file>
@@ -437,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A67"/>
+  <dimension ref="A1:A79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -783,6 +804,66 @@
         <v>16</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Prueba remote de test RUN FIREFOX (intellij Idea)
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="25">
   <si>
     <t>$ 27.323 CLP 17-10-20</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>$ 27.515 CLP 20-11-20</t>
+  </si>
+  <si>
+    <t>$ 27.534 CLP 23-11-20</t>
   </si>
 </sst>
 </file>
@@ -458,7 +461,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A79"/>
+  <dimension ref="A1:A81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -864,6 +867,16 @@
         <v>23</v>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Run en Firefox (Producto)
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="28">
   <si>
     <t>$ 27.323 CLP 17-10-20</t>
   </si>
@@ -470,7 +470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A96"/>
+  <dimension ref="A1:A97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -961,6 +961,11 @@
         <v>26</v>
       </c>
     </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Run en Firefox prueba MENSAJES
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhurtado\Documents\QA Gestion Corredor\Toctoc_QA_Gestion_Corredor\src\test\resources\filepath\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2531B6-6D7C-4BC9-A272-BCBC4859DBA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87904BCD-3DE0-4725-B595-B0B7F15A7DEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1A15881D-BF6E-4E61-BDC0-2AE68B47EA9A}"/>
+    <workbookView xWindow="-20490" yWindow="3630" windowWidth="17280" windowHeight="8970" xr2:uid="{1A15881D-BF6E-4E61-BDC0-2AE68B47EA9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="34">
   <si>
     <t>$ 27.323 CLP 17-10-20</t>
   </si>
@@ -118,6 +118,24 @@
   </si>
   <si>
     <t>$ 34.618 CLP 09-12-20</t>
+  </si>
+  <si>
+    <t>$ 27.629 CLP 17-12-20</t>
+  </si>
+  <si>
+    <t>$ 27.628 CLP 18-12-20</t>
+  </si>
+  <si>
+    <t>$ 27.626 CLP 21-12-20</t>
+  </si>
+  <si>
+    <t>$ 34.604 CLP 22-12-20</t>
+  </si>
+  <si>
+    <t>$ 34.596 CLP 29-12-20</t>
+  </si>
+  <si>
+    <t>$ 27.619 CLP 29-12-20</t>
   </si>
 </sst>
 </file>
@@ -470,15 +488,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A97"/>
+  <dimension ref="A1:A105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="38.6640625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="41.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -806,164 +824,204 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run en Firefox Actualización de localizador
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="38">
   <si>
     <t>$ 27.323 CLP 17-10-20</t>
   </si>
@@ -136,6 +136,18 @@
   </si>
   <si>
     <t>$ 27.619 CLP 29-12-20</t>
+  </si>
+  <si>
+    <t>$ 27.617 CLP 31-12-20</t>
+  </si>
+  <si>
+    <t>$ 27.613 CLP 04-01-21</t>
+  </si>
+  <si>
+    <t>$ 34.589 CLP 04-01-21</t>
+  </si>
+  <si>
+    <t>0.95 UF 13-01-21</t>
   </si>
 </sst>
 </file>
@@ -488,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A105"/>
+  <dimension ref="A1:A113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
       <selection activeCell="A103" sqref="A103"/>
@@ -1024,6 +1036,46 @@
         <v>33</v>
       </c>
     </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>